<commit_message>
Excel Template 更新,43010,43020 EWMA顯示資料欄位調整
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/40040.xlsx
+++ b/PhoenixCI/Excel_Template/40040.xlsx
@@ -2422,6 +2422,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2446,9 +2452,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2533,11 +2536,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2849,16 +2849,19 @@
   </sheetPr>
   <dimension ref="B1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" activeCellId="2" sqref="D7:D41 F7:F41 H7:H41"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="1" style="40" customWidth="1"/>
     <col min="2" max="2" width="9.375" style="65" customWidth="1"/>
-    <col min="3" max="6" width="12.375" style="48" customWidth="1"/>
-    <col min="7" max="7" width="12.375" style="40" customWidth="1"/>
+    <col min="3" max="3" width="11.625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="12.375" style="48" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="12.375" style="48" customWidth="1"/>
+    <col min="7" max="7" width="11.625" style="40" customWidth="1"/>
     <col min="8" max="8" width="12.375" style="49" customWidth="1"/>
     <col min="9" max="9" width="10.25" style="49" customWidth="1"/>
     <col min="10" max="10" width="11.875" style="48" customWidth="1"/>
@@ -2871,12 +2874,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19">
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="113"/>
+      <c r="P1" s="113"/>
+      <c r="Q1" s="113"/>
+      <c r="R1" s="113"/>
+      <c r="S1" s="113"/>
     </row>
     <row r="2" spans="2:19" ht="6.75" customHeight="1"/>
     <row r="3" spans="2:19" ht="16.5">
@@ -2888,71 +2891,71 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="20.25" customHeight="1">
-      <c r="B4" s="87"/>
-      <c r="C4" s="88" t="s">
+      <c r="B4" s="88"/>
+      <c r="C4" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="84" t="s">
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="85" t="s">
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="M4" s="86"/>
-      <c r="N4" s="84" t="s">
+      <c r="M4" s="87"/>
+      <c r="N4" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="85"/>
     </row>
     <row r="5" spans="2:19" ht="34.5" customHeight="1">
-      <c r="B5" s="87"/>
-      <c r="C5" s="77" t="s">
+      <c r="B5" s="88"/>
+      <c r="C5" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="77" t="s">
+      <c r="D5" s="80"/>
+      <c r="E5" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="F5" s="78"/>
-      <c r="G5" s="77" t="s">
+      <c r="F5" s="80"/>
+      <c r="G5" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="77" t="s">
+      <c r="H5" s="80"/>
+      <c r="I5" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78" t="s">
+      <c r="J5" s="80"/>
+      <c r="K5" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="79" t="s">
+      <c r="L5" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="M5" s="79" t="s">
+      <c r="M5" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="N5" s="77" t="s">
+      <c r="N5" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-      <c r="S5" s="78"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
     </row>
     <row r="6" spans="2:19" ht="63">
-      <c r="B6" s="87"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="63" t="s">
         <v>89</v>
       </c>
@@ -2977,9 +2980,9 @@
       <c r="J6" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="K6" s="78"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
       <c r="N6" s="72" t="s">
         <v>111</v>
       </c>
@@ -3004,11 +3007,11 @@
         <v>0</v>
       </c>
       <c r="C7" s="32"/>
-      <c r="D7" s="112"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="32"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="112"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="34"/>
       <c r="J7" s="35"/>
       <c r="K7" s="31"/>
@@ -3028,11 +3031,11 @@
         <v>1</v>
       </c>
       <c r="C8" s="32"/>
-      <c r="D8" s="112"/>
+      <c r="D8" s="75"/>
       <c r="E8" s="32"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="112"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="34"/>
       <c r="J8" s="35"/>
       <c r="K8" s="31"/>
@@ -3050,11 +3053,11 @@
         <v>2</v>
       </c>
       <c r="C9" s="32"/>
-      <c r="D9" s="112"/>
+      <c r="D9" s="75"/>
       <c r="E9" s="32"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="112"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="34"/>
       <c r="J9" s="35"/>
       <c r="K9" s="31"/>
@@ -3072,11 +3075,11 @@
         <v>3</v>
       </c>
       <c r="C10" s="32"/>
-      <c r="D10" s="112"/>
+      <c r="D10" s="75"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="112"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="34"/>
       <c r="J10" s="35"/>
       <c r="K10" s="31"/>
@@ -3094,11 +3097,11 @@
         <v>4</v>
       </c>
       <c r="C11" s="32"/>
-      <c r="D11" s="112"/>
+      <c r="D11" s="75"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="112"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="75"/>
       <c r="I11" s="34"/>
       <c r="J11" s="35"/>
       <c r="K11" s="31"/>
@@ -3116,11 +3119,11 @@
         <v>10</v>
       </c>
       <c r="C12" s="32"/>
-      <c r="D12" s="112"/>
+      <c r="D12" s="75"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="112"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="75"/>
       <c r="I12" s="34"/>
       <c r="J12" s="35"/>
       <c r="K12" s="31"/>
@@ -3138,11 +3141,11 @@
         <v>11</v>
       </c>
       <c r="C13" s="32"/>
-      <c r="D13" s="112"/>
+      <c r="D13" s="75"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="112"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="75"/>
       <c r="I13" s="34"/>
       <c r="J13" s="35"/>
       <c r="K13" s="31"/>
@@ -3160,11 +3163,11 @@
         <v>12</v>
       </c>
       <c r="C14" s="32"/>
-      <c r="D14" s="112"/>
+      <c r="D14" s="75"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="112"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="75"/>
       <c r="I14" s="34"/>
       <c r="J14" s="35"/>
       <c r="K14" s="31"/>
@@ -3182,11 +3185,11 @@
         <v>51</v>
       </c>
       <c r="C15" s="32"/>
-      <c r="D15" s="112"/>
+      <c r="D15" s="75"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="112"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="75"/>
       <c r="I15" s="34"/>
       <c r="J15" s="35"/>
       <c r="K15" s="31"/>
@@ -3204,11 +3207,11 @@
         <v>13</v>
       </c>
       <c r="C16" s="32"/>
-      <c r="D16" s="112"/>
+      <c r="D16" s="75"/>
       <c r="E16" s="32"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="112"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="34"/>
       <c r="J16" s="35"/>
       <c r="K16" s="31"/>
@@ -3226,11 +3229,11 @@
         <v>47</v>
       </c>
       <c r="C17" s="32"/>
-      <c r="D17" s="112"/>
+      <c r="D17" s="75"/>
       <c r="E17" s="32"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="112"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="75"/>
       <c r="I17" s="34"/>
       <c r="J17" s="35"/>
       <c r="K17" s="31"/>
@@ -3248,11 +3251,11 @@
         <v>71</v>
       </c>
       <c r="C18" s="37"/>
-      <c r="D18" s="112"/>
+      <c r="D18" s="75"/>
       <c r="E18" s="37"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="113"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="76"/>
       <c r="I18" s="38"/>
       <c r="J18" s="39"/>
       <c r="K18" s="47"/>
@@ -3270,11 +3273,11 @@
         <v>75</v>
       </c>
       <c r="C19" s="37"/>
-      <c r="D19" s="112"/>
+      <c r="D19" s="75"/>
       <c r="E19" s="37"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="113"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="76"/>
       <c r="I19" s="38"/>
       <c r="J19" s="39"/>
       <c r="K19" s="47"/>
@@ -3292,11 +3295,11 @@
         <v>76</v>
       </c>
       <c r="C20" s="37"/>
-      <c r="D20" s="112"/>
+      <c r="D20" s="75"/>
       <c r="E20" s="37"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="113"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="76"/>
       <c r="I20" s="38"/>
       <c r="J20" s="39"/>
       <c r="K20" s="47"/>
@@ -3314,11 +3317,11 @@
         <v>80</v>
       </c>
       <c r="C21" s="37"/>
-      <c r="D21" s="112"/>
+      <c r="D21" s="75"/>
       <c r="E21" s="37"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="113"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="76"/>
       <c r="I21" s="38"/>
       <c r="J21" s="39"/>
       <c r="K21" s="47"/>
@@ -3336,11 +3339,11 @@
         <v>81</v>
       </c>
       <c r="C22" s="37"/>
-      <c r="D22" s="112"/>
+      <c r="D22" s="75"/>
       <c r="E22" s="37"/>
-      <c r="F22" s="112"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="113"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="76"/>
       <c r="I22" s="38"/>
       <c r="J22" s="39"/>
       <c r="K22" s="47"/>
@@ -3358,11 +3361,11 @@
         <v>45</v>
       </c>
       <c r="C23" s="32"/>
-      <c r="D23" s="112"/>
+      <c r="D23" s="75"/>
       <c r="E23" s="32"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="112"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="34"/>
       <c r="J23" s="35"/>
       <c r="K23" s="31"/>
@@ -3380,11 +3383,11 @@
         <v>46</v>
       </c>
       <c r="C24" s="32"/>
-      <c r="D24" s="112"/>
+      <c r="D24" s="75"/>
       <c r="E24" s="32"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="112"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="75"/>
       <c r="I24" s="34"/>
       <c r="J24" s="35"/>
       <c r="K24" s="31"/>
@@ -3402,11 +3405,11 @@
         <v>69</v>
       </c>
       <c r="C25" s="37"/>
-      <c r="D25" s="112"/>
+      <c r="D25" s="75"/>
       <c r="E25" s="37"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="113"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="76"/>
       <c r="I25" s="38"/>
       <c r="J25" s="39"/>
       <c r="K25" s="47"/>
@@ -3424,11 +3427,11 @@
         <v>70</v>
       </c>
       <c r="C26" s="37"/>
-      <c r="D26" s="112"/>
+      <c r="D26" s="75"/>
       <c r="E26" s="37"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="113"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="76"/>
       <c r="I26" s="38"/>
       <c r="J26" s="39"/>
       <c r="K26" s="47"/>
@@ -3446,11 +3449,11 @@
         <v>77</v>
       </c>
       <c r="C27" s="32"/>
-      <c r="D27" s="112"/>
+      <c r="D27" s="75"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="112"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="75"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
       <c r="K27" s="31"/>
@@ -3468,11 +3471,11 @@
         <v>78</v>
       </c>
       <c r="C28" s="32"/>
-      <c r="D28" s="112"/>
+      <c r="D28" s="75"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="112"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="112"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="75"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
       <c r="K28" s="31"/>
@@ -3490,11 +3493,11 @@
         <v>14</v>
       </c>
       <c r="C29" s="32"/>
-      <c r="D29" s="112"/>
+      <c r="D29" s="75"/>
       <c r="E29" s="32"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="112"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="75"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
       <c r="K29" s="31"/>
@@ -3512,11 +3515,11 @@
         <v>90</v>
       </c>
       <c r="C30" s="64"/>
-      <c r="D30" s="112"/>
+      <c r="D30" s="75"/>
       <c r="E30" s="64"/>
-      <c r="F30" s="112"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="112"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="75"/>
       <c r="I30" s="61"/>
       <c r="J30" s="35"/>
       <c r="K30" s="59"/>
@@ -3534,11 +3537,11 @@
         <v>15</v>
       </c>
       <c r="C31" s="32"/>
-      <c r="D31" s="112"/>
+      <c r="D31" s="75"/>
       <c r="E31" s="32"/>
-      <c r="F31" s="112"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="112"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="75"/>
       <c r="I31" s="34"/>
       <c r="J31" s="35"/>
       <c r="K31" s="31"/>
@@ -3556,11 +3559,11 @@
         <v>91</v>
       </c>
       <c r="C32" s="64"/>
-      <c r="D32" s="112"/>
+      <c r="D32" s="75"/>
       <c r="E32" s="64"/>
-      <c r="F32" s="112"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="112"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="75"/>
       <c r="I32" s="61"/>
       <c r="J32" s="35"/>
       <c r="K32" s="59"/>
@@ -3578,11 +3581,11 @@
         <v>16</v>
       </c>
       <c r="C33" s="32"/>
-      <c r="D33" s="112"/>
+      <c r="D33" s="75"/>
       <c r="E33" s="32"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="112"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="75"/>
       <c r="I33" s="34"/>
       <c r="J33" s="35"/>
       <c r="K33" s="31"/>
@@ -3600,11 +3603,11 @@
         <v>92</v>
       </c>
       <c r="C34" s="64"/>
-      <c r="D34" s="112"/>
+      <c r="D34" s="75"/>
       <c r="E34" s="64"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="112"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="64"/>
+      <c r="H34" s="75"/>
       <c r="I34" s="61"/>
       <c r="J34" s="35"/>
       <c r="K34" s="59"/>
@@ -3622,11 +3625,11 @@
         <v>17</v>
       </c>
       <c r="C35" s="32"/>
-      <c r="D35" s="112"/>
+      <c r="D35" s="75"/>
       <c r="E35" s="32"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="112"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="75"/>
       <c r="I35" s="34"/>
       <c r="J35" s="35"/>
       <c r="K35" s="31"/>
@@ -3644,11 +3647,11 @@
         <v>93</v>
       </c>
       <c r="C36" s="64"/>
-      <c r="D36" s="112"/>
+      <c r="D36" s="75"/>
       <c r="E36" s="64"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="112"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="75"/>
       <c r="I36" s="61"/>
       <c r="J36" s="35"/>
       <c r="K36" s="59"/>
@@ -3666,11 +3669,11 @@
         <v>18</v>
       </c>
       <c r="C37" s="32"/>
-      <c r="D37" s="112"/>
+      <c r="D37" s="75"/>
       <c r="E37" s="32"/>
-      <c r="F37" s="112"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="112"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="75"/>
       <c r="I37" s="34"/>
       <c r="J37" s="35"/>
       <c r="K37" s="31"/>
@@ -3688,11 +3691,11 @@
         <v>94</v>
       </c>
       <c r="C38" s="64"/>
-      <c r="D38" s="112"/>
+      <c r="D38" s="75"/>
       <c r="E38" s="64"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="112"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="75"/>
       <c r="I38" s="61"/>
       <c r="J38" s="35"/>
       <c r="K38" s="59"/>
@@ -3710,11 +3713,11 @@
         <v>19</v>
       </c>
       <c r="C39" s="32"/>
-      <c r="D39" s="112"/>
+      <c r="D39" s="75"/>
       <c r="E39" s="32"/>
-      <c r="F39" s="112"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="112"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="34"/>
       <c r="J39" s="35"/>
       <c r="K39" s="31"/>
@@ -3732,11 +3735,11 @@
         <v>48</v>
       </c>
       <c r="C40" s="32"/>
-      <c r="D40" s="112"/>
+      <c r="D40" s="75"/>
       <c r="E40" s="32"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="112"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="64"/>
+      <c r="H40" s="75"/>
       <c r="I40" s="34"/>
       <c r="J40" s="35"/>
       <c r="K40" s="31"/>
@@ -3754,11 +3757,11 @@
         <v>49</v>
       </c>
       <c r="C41" s="32"/>
-      <c r="D41" s="112"/>
+      <c r="D41" s="75"/>
       <c r="E41" s="32"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="112"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="75"/>
       <c r="I41" s="34"/>
       <c r="J41" s="35"/>
       <c r="K41" s="31"/>
@@ -3777,20 +3780,20 @@
       </c>
     </row>
     <row r="43" spans="2:19" ht="16.5">
-      <c r="B43" s="81" t="s">
+      <c r="B43" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C43" s="82"/>
-      <c r="D43" s="82"/>
-      <c r="E43" s="82"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="82"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="82"/>
-      <c r="K43" s="82"/>
-      <c r="L43" s="82"/>
-      <c r="M43" s="82"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="84"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="84"/>
+      <c r="I43" s="84"/>
+      <c r="J43" s="84"/>
+      <c r="K43" s="84"/>
+      <c r="L43" s="84"/>
+      <c r="M43" s="84"/>
     </row>
     <row r="44" spans="2:19" ht="16.5">
       <c r="B44" s="60" t="s">
@@ -3814,18 +3817,18 @@
       <c r="B49" s="73">
         <v>1</v>
       </c>
-      <c r="C49" s="75" t="s">
+      <c r="C49" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="76"/>
-      <c r="E49" s="76"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="76"/>
-      <c r="I49" s="76"/>
-      <c r="J49" s="76"/>
-      <c r="K49" s="76"/>
-      <c r="L49" s="76"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="78"/>
+      <c r="F49" s="78"/>
+      <c r="G49" s="78"/>
+      <c r="H49" s="78"/>
+      <c r="I49" s="78"/>
+      <c r="J49" s="78"/>
+      <c r="K49" s="78"/>
+      <c r="L49" s="78"/>
     </row>
     <row r="50" spans="2:12" ht="16.5">
       <c r="B50" s="73">
@@ -3976,16 +3979,16 @@
     </row>
     <row r="61" spans="2:12">
       <c r="B61" s="69"/>
-      <c r="C61" s="75"/>
-      <c r="D61" s="76"/>
-      <c r="E61" s="76"/>
-      <c r="F61" s="76"/>
-      <c r="G61" s="76"/>
-      <c r="H61" s="76"/>
-      <c r="I61" s="76"/>
-      <c r="J61" s="76"/>
-      <c r="K61" s="76"/>
-      <c r="L61" s="76"/>
+      <c r="C61" s="77"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="78"/>
+      <c r="F61" s="78"/>
+      <c r="G61" s="78"/>
+      <c r="H61" s="78"/>
+      <c r="I61" s="78"/>
+      <c r="J61" s="78"/>
+      <c r="K61" s="78"/>
+      <c r="L61" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -4023,8 +4026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J56"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4035,22 +4038,23 @@
     <col min="4" max="4" width="12.25" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.25" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.75" style="10" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="10" customWidth="1"/>
-    <col min="9" max="10" width="10.125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="15.375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8.5" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="9.625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="11.875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="9.625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="11.875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.625" style="16" customWidth="1"/>
     <col min="13" max="13" width="10.25" style="16" customWidth="1"/>
-    <col min="14" max="14" width="11.875" style="10" customWidth="1"/>
+    <col min="14" max="14" width="9.75" style="10" customWidth="1"/>
     <col min="15" max="15" width="8" style="3" customWidth="1"/>
     <col min="16" max="17" width="13.875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="P1" s="91" t="s">
+      <c r="P1" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="91"/>
+      <c r="Q1" s="92"/>
     </row>
     <row r="2" spans="1:17" ht="6.75" customHeight="1"/>
     <row r="3" spans="1:17" s="1" customFormat="1">
@@ -4078,77 +4082,77 @@
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="20.25" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="95" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="20"/>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="84" t="s">
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="78" t="s">
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="Q4" s="78"/>
+      <c r="Q4" s="80"/>
     </row>
     <row r="5" spans="1:17" ht="31.9" customHeight="1">
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="94" t="s">
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="77" t="s">
+      <c r="H5" s="80"/>
+      <c r="I5" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="78"/>
-      <c r="K5" s="77" t="s">
+      <c r="J5" s="80"/>
+      <c r="K5" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="L5" s="78"/>
-      <c r="M5" s="77" t="s">
+      <c r="L5" s="80"/>
+      <c r="M5" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78" t="s">
+      <c r="N5" s="80"/>
+      <c r="O5" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="79" t="s">
+      <c r="P5" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="Q5" s="79" t="s">
+      <c r="Q5" s="81" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="54" customHeight="1">
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
+      <c r="B6" s="97"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
       <c r="G6" s="63" t="s">
         <v>89</v>
       </c>
@@ -4173,9 +4177,9 @@
       <c r="N6" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="O6" s="78"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
     </row>
     <row r="7" spans="1:17" s="14" customFormat="1">
       <c r="A7" s="11"/>
@@ -4185,11 +4189,11 @@
       <c r="E7" s="25"/>
       <c r="F7" s="26"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="17"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="17"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="75"/>
       <c r="M7" s="17"/>
       <c r="N7" s="19"/>
       <c r="O7" s="12"/>
@@ -4204,11 +4208,11 @@
       <c r="E8" s="25"/>
       <c r="F8" s="26"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="17"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="17"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="75"/>
       <c r="M8" s="17"/>
       <c r="N8" s="19"/>
       <c r="O8" s="12"/>
@@ -4223,11 +4227,11 @@
       <c r="E9" s="25"/>
       <c r="F9" s="26"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="17"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="17"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="75"/>
       <c r="M9" s="17"/>
       <c r="N9" s="19"/>
       <c r="O9" s="12"/>
@@ -4242,11 +4246,11 @@
       <c r="E10" s="25"/>
       <c r="F10" s="26"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="17"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="17"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="75"/>
       <c r="M10" s="17"/>
       <c r="N10" s="19"/>
       <c r="O10" s="12"/>
@@ -4261,11 +4265,11 @@
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="17"/>
+      <c r="H11" s="75"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="17"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="75"/>
       <c r="M11" s="17"/>
       <c r="N11" s="19"/>
       <c r="O11" s="12"/>
@@ -4280,11 +4284,11 @@
       <c r="E12" s="25"/>
       <c r="F12" s="26"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="17"/>
+      <c r="H12" s="75"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="17"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="75"/>
       <c r="M12" s="17"/>
       <c r="N12" s="19"/>
       <c r="O12" s="12"/>
@@ -4299,11 +4303,11 @@
       <c r="E13" s="25"/>
       <c r="F13" s="26"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="75"/>
       <c r="I13" s="13"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="17"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="75"/>
       <c r="M13" s="17"/>
       <c r="N13" s="19"/>
       <c r="O13" s="12"/>
@@ -4318,11 +4322,11 @@
       <c r="E14" s="25"/>
       <c r="F14" s="26"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="75"/>
       <c r="I14" s="13"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="17"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="75"/>
       <c r="M14" s="17"/>
       <c r="N14" s="19"/>
       <c r="O14" s="12"/>
@@ -4337,11 +4341,11 @@
       <c r="E15" s="25"/>
       <c r="F15" s="26"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="17"/>
+      <c r="H15" s="75"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="17"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="75"/>
       <c r="M15" s="17"/>
       <c r="N15" s="19"/>
       <c r="O15" s="12"/>
@@ -4356,11 +4360,11 @@
       <c r="E16" s="25"/>
       <c r="F16" s="26"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="17"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="13"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="17"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="75"/>
       <c r="M16" s="17"/>
       <c r="N16" s="19"/>
       <c r="O16" s="12"/>
@@ -4375,11 +4379,11 @@
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="17"/>
+      <c r="H17" s="75"/>
       <c r="I17" s="13"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="17"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="75"/>
       <c r="M17" s="17"/>
       <c r="N17" s="19"/>
       <c r="O17" s="12"/>
@@ -4394,11 +4398,11 @@
       <c r="E18" s="25"/>
       <c r="F18" s="26"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="17"/>
+      <c r="H18" s="75"/>
       <c r="I18" s="13"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="17"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="75"/>
       <c r="M18" s="17"/>
       <c r="N18" s="19"/>
       <c r="O18" s="12"/>
@@ -4413,11 +4417,11 @@
       <c r="E19" s="25"/>
       <c r="F19" s="26"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="17"/>
+      <c r="H19" s="75"/>
       <c r="I19" s="13"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="17"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="75"/>
       <c r="M19" s="17"/>
       <c r="N19" s="19"/>
       <c r="O19" s="12"/>
@@ -4432,11 +4436,11 @@
       <c r="E20" s="25"/>
       <c r="F20" s="26"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="75"/>
       <c r="I20" s="13"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="17"/>
+      <c r="J20" s="75"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="75"/>
       <c r="M20" s="17"/>
       <c r="N20" s="19"/>
       <c r="O20" s="12"/>
@@ -4451,11 +4455,11 @@
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="17"/>
+      <c r="H21" s="75"/>
       <c r="I21" s="13"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="17"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="75"/>
       <c r="M21" s="17"/>
       <c r="N21" s="19"/>
       <c r="O21" s="12"/>
@@ -4470,11 +4474,11 @@
       <c r="E22" s="25"/>
       <c r="F22" s="26"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="17"/>
+      <c r="H22" s="75"/>
       <c r="I22" s="13"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="17"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="75"/>
       <c r="M22" s="17"/>
       <c r="N22" s="19"/>
       <c r="O22" s="12"/>
@@ -4489,11 +4493,11 @@
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="17"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="13"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="17"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="75"/>
       <c r="M23" s="17"/>
       <c r="N23" s="19"/>
       <c r="O23" s="12"/>
@@ -4508,11 +4512,11 @@
       <c r="E24" s="25"/>
       <c r="F24" s="26"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="17"/>
+      <c r="H24" s="75"/>
       <c r="I24" s="13"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="17"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="75"/>
       <c r="M24" s="17"/>
       <c r="N24" s="19"/>
       <c r="O24" s="12"/>
@@ -4527,11 +4531,11 @@
       <c r="E25" s="25"/>
       <c r="F25" s="26"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="17"/>
+      <c r="H25" s="75"/>
       <c r="I25" s="13"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="17"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="75"/>
       <c r="M25" s="17"/>
       <c r="N25" s="19"/>
       <c r="O25" s="12"/>
@@ -4546,11 +4550,11 @@
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="75"/>
       <c r="I26" s="13"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="17"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="75"/>
       <c r="M26" s="17"/>
       <c r="N26" s="19"/>
       <c r="O26" s="12"/>
@@ -4565,11 +4569,11 @@
       <c r="E27" s="25"/>
       <c r="F27" s="26"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="17"/>
+      <c r="H27" s="75"/>
       <c r="I27" s="13"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="17"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="75"/>
       <c r="M27" s="17"/>
       <c r="N27" s="19"/>
       <c r="O27" s="12"/>
@@ -4584,11 +4588,11 @@
       <c r="E28" s="25"/>
       <c r="F28" s="26"/>
       <c r="G28" s="13"/>
-      <c r="H28" s="17"/>
+      <c r="H28" s="75"/>
       <c r="I28" s="13"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="17"/>
+      <c r="J28" s="75"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="75"/>
       <c r="M28" s="17"/>
       <c r="N28" s="19"/>
       <c r="O28" s="12"/>
@@ -4603,11 +4607,11 @@
       <c r="E29" s="25"/>
       <c r="F29" s="26"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="17"/>
+      <c r="H29" s="75"/>
       <c r="I29" s="13"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="17"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="75"/>
       <c r="M29" s="17"/>
       <c r="N29" s="19"/>
       <c r="O29" s="12"/>
@@ -4622,11 +4626,11 @@
       <c r="E30" s="25"/>
       <c r="F30" s="26"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="17"/>
+      <c r="H30" s="75"/>
       <c r="I30" s="13"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="17"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="75"/>
       <c r="M30" s="17"/>
       <c r="N30" s="19"/>
       <c r="O30" s="12"/>
@@ -4641,11 +4645,11 @@
       <c r="E31" s="25"/>
       <c r="F31" s="26"/>
       <c r="G31" s="13"/>
-      <c r="H31" s="17"/>
+      <c r="H31" s="75"/>
       <c r="I31" s="13"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="17"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="75"/>
       <c r="M31" s="17"/>
       <c r="N31" s="19"/>
       <c r="O31" s="12"/>
@@ -4660,11 +4664,11 @@
       <c r="E32" s="25"/>
       <c r="F32" s="26"/>
       <c r="G32" s="13"/>
-      <c r="H32" s="17"/>
+      <c r="H32" s="75"/>
       <c r="I32" s="13"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="17"/>
+      <c r="J32" s="75"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="75"/>
       <c r="M32" s="17"/>
       <c r="N32" s="19"/>
       <c r="O32" s="12"/>
@@ -4679,11 +4683,11 @@
       <c r="E33" s="25"/>
       <c r="F33" s="26"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="17"/>
+      <c r="H33" s="75"/>
       <c r="I33" s="13"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="17"/>
+      <c r="J33" s="75"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="75"/>
       <c r="M33" s="17"/>
       <c r="N33" s="19"/>
       <c r="O33" s="12"/>
@@ -4698,11 +4702,11 @@
       <c r="E34" s="25"/>
       <c r="F34" s="26"/>
       <c r="G34" s="13"/>
-      <c r="H34" s="17"/>
+      <c r="H34" s="75"/>
       <c r="I34" s="13"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="17"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="75"/>
       <c r="M34" s="17"/>
       <c r="N34" s="19"/>
       <c r="O34" s="12"/>
@@ -4717,11 +4721,11 @@
       <c r="E35" s="25"/>
       <c r="F35" s="26"/>
       <c r="G35" s="13"/>
-      <c r="H35" s="17"/>
+      <c r="H35" s="75"/>
       <c r="I35" s="13"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="17"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="75"/>
       <c r="M35" s="17"/>
       <c r="N35" s="19"/>
       <c r="O35" s="12"/>
@@ -4736,11 +4740,11 @@
       <c r="E36" s="25"/>
       <c r="F36" s="26"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="17"/>
+      <c r="H36" s="75"/>
       <c r="I36" s="13"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="17"/>
+      <c r="J36" s="75"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="75"/>
       <c r="M36" s="17"/>
       <c r="N36" s="19"/>
       <c r="O36" s="12"/>
@@ -4755,11 +4759,11 @@
       <c r="E37" s="25"/>
       <c r="F37" s="26"/>
       <c r="G37" s="13"/>
-      <c r="H37" s="17"/>
+      <c r="H37" s="75"/>
       <c r="I37" s="13"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="17"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="75"/>
       <c r="M37" s="17"/>
       <c r="N37" s="19"/>
       <c r="O37" s="12"/>
@@ -4774,11 +4778,11 @@
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="13"/>
-      <c r="H38" s="17"/>
+      <c r="H38" s="75"/>
       <c r="I38" s="13"/>
-      <c r="J38" s="17"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="17"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="75"/>
       <c r="M38" s="17"/>
       <c r="N38" s="19"/>
       <c r="O38" s="12"/>
@@ -4793,11 +4797,11 @@
       <c r="E39" s="25"/>
       <c r="F39" s="26"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="17"/>
+      <c r="H39" s="75"/>
       <c r="I39" s="13"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="17"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="75"/>
       <c r="M39" s="17"/>
       <c r="N39" s="19"/>
       <c r="O39" s="12"/>
@@ -4812,11 +4816,11 @@
       <c r="E40" s="25"/>
       <c r="F40" s="26"/>
       <c r="G40" s="13"/>
-      <c r="H40" s="17"/>
+      <c r="H40" s="75"/>
       <c r="I40" s="13"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="17"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="75"/>
       <c r="M40" s="17"/>
       <c r="N40" s="19"/>
       <c r="O40" s="12"/>
@@ -4831,11 +4835,11 @@
       <c r="E41" s="25"/>
       <c r="F41" s="26"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="17"/>
+      <c r="H41" s="75"/>
       <c r="I41" s="13"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="17"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="13"/>
+      <c r="L41" s="75"/>
       <c r="M41" s="17"/>
       <c r="N41" s="19"/>
       <c r="O41" s="12"/>
@@ -4850,11 +4854,11 @@
       <c r="E42" s="25"/>
       <c r="F42" s="26"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="17"/>
+      <c r="H42" s="75"/>
       <c r="I42" s="13"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="17"/>
+      <c r="J42" s="75"/>
+      <c r="K42" s="13"/>
+      <c r="L42" s="75"/>
       <c r="M42" s="17"/>
       <c r="N42" s="19"/>
       <c r="O42" s="12"/>
@@ -4869,11 +4873,11 @@
       <c r="E43" s="25"/>
       <c r="F43" s="26"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="17"/>
+      <c r="H43" s="75"/>
       <c r="I43" s="13"/>
-      <c r="J43" s="17"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="17"/>
+      <c r="J43" s="75"/>
+      <c r="K43" s="13"/>
+      <c r="L43" s="75"/>
       <c r="M43" s="17"/>
       <c r="N43" s="19"/>
       <c r="O43" s="12"/>
@@ -4888,11 +4892,11 @@
       <c r="E44" s="25"/>
       <c r="F44" s="26"/>
       <c r="G44" s="13"/>
-      <c r="H44" s="17"/>
+      <c r="H44" s="75"/>
       <c r="I44" s="13"/>
-      <c r="J44" s="17"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="17"/>
+      <c r="J44" s="75"/>
+      <c r="K44" s="13"/>
+      <c r="L44" s="75"/>
       <c r="M44" s="17"/>
       <c r="N44" s="19"/>
       <c r="O44" s="12"/>
@@ -4907,11 +4911,11 @@
       <c r="E45" s="25"/>
       <c r="F45" s="26"/>
       <c r="G45" s="13"/>
-      <c r="H45" s="17"/>
+      <c r="H45" s="75"/>
       <c r="I45" s="13"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="17"/>
+      <c r="J45" s="75"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="75"/>
       <c r="M45" s="17"/>
       <c r="N45" s="19"/>
       <c r="O45" s="12"/>
@@ -4926,11 +4930,11 @@
       <c r="E46" s="25"/>
       <c r="F46" s="26"/>
       <c r="G46" s="13"/>
-      <c r="H46" s="17"/>
+      <c r="H46" s="75"/>
       <c r="I46" s="13"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="17"/>
+      <c r="J46" s="75"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="75"/>
       <c r="M46" s="17"/>
       <c r="N46" s="19"/>
       <c r="O46" s="12"/>
@@ -4945,11 +4949,11 @@
       <c r="E47" s="25"/>
       <c r="F47" s="26"/>
       <c r="G47" s="13"/>
-      <c r="H47" s="17"/>
+      <c r="H47" s="75"/>
       <c r="I47" s="13"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="17"/>
+      <c r="J47" s="75"/>
+      <c r="K47" s="13"/>
+      <c r="L47" s="75"/>
       <c r="M47" s="17"/>
       <c r="N47" s="19"/>
       <c r="O47" s="12"/>
@@ -4964,11 +4968,11 @@
       <c r="E48" s="25"/>
       <c r="F48" s="26"/>
       <c r="G48" s="13"/>
-      <c r="H48" s="17"/>
+      <c r="H48" s="75"/>
       <c r="I48" s="13"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="17"/>
+      <c r="J48" s="75"/>
+      <c r="K48" s="13"/>
+      <c r="L48" s="75"/>
       <c r="M48" s="17"/>
       <c r="N48" s="19"/>
       <c r="O48" s="12"/>
@@ -4983,11 +4987,11 @@
       <c r="E49" s="25"/>
       <c r="F49" s="26"/>
       <c r="G49" s="13"/>
-      <c r="H49" s="17"/>
+      <c r="H49" s="75"/>
       <c r="I49" s="13"/>
-      <c r="J49" s="17"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="17"/>
+      <c r="J49" s="75"/>
+      <c r="K49" s="13"/>
+      <c r="L49" s="75"/>
       <c r="M49" s="17"/>
       <c r="N49" s="19"/>
       <c r="O49" s="12"/>
@@ -5002,11 +5006,11 @@
       <c r="E50" s="25"/>
       <c r="F50" s="26"/>
       <c r="G50" s="13"/>
-      <c r="H50" s="17"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="13"/>
-      <c r="J50" s="17"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="17"/>
+      <c r="J50" s="75"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="75"/>
       <c r="M50" s="17"/>
       <c r="N50" s="19"/>
       <c r="O50" s="12"/>
@@ -5021,11 +5025,11 @@
       <c r="E51" s="25"/>
       <c r="F51" s="26"/>
       <c r="G51" s="13"/>
-      <c r="H51" s="17"/>
+      <c r="H51" s="75"/>
       <c r="I51" s="13"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="17"/>
+      <c r="J51" s="75"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="75"/>
       <c r="M51" s="17"/>
       <c r="N51" s="19"/>
       <c r="O51" s="12"/>
@@ -5040,11 +5044,11 @@
       <c r="E52" s="25"/>
       <c r="F52" s="26"/>
       <c r="G52" s="13"/>
-      <c r="H52" s="17"/>
+      <c r="H52" s="75"/>
       <c r="I52" s="13"/>
-      <c r="J52" s="17"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="17"/>
+      <c r="J52" s="75"/>
+      <c r="K52" s="13"/>
+      <c r="L52" s="75"/>
       <c r="M52" s="17"/>
       <c r="N52" s="19"/>
       <c r="O52" s="12"/>
@@ -5059,11 +5063,11 @@
       <c r="E53" s="25"/>
       <c r="F53" s="26"/>
       <c r="G53" s="13"/>
-      <c r="H53" s="17"/>
+      <c r="H53" s="75"/>
       <c r="I53" s="13"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="17"/>
+      <c r="J53" s="75"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="75"/>
       <c r="M53" s="17"/>
       <c r="N53" s="19"/>
       <c r="O53" s="12"/>
@@ -5078,11 +5082,11 @@
       <c r="E54" s="25"/>
       <c r="F54" s="26"/>
       <c r="G54" s="13"/>
-      <c r="H54" s="17"/>
+      <c r="H54" s="75"/>
       <c r="I54" s="13"/>
-      <c r="J54" s="17"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="17"/>
+      <c r="J54" s="75"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="75"/>
       <c r="M54" s="17"/>
       <c r="N54" s="19"/>
       <c r="O54" s="12"/>
@@ -5097,11 +5101,11 @@
       <c r="E55" s="25"/>
       <c r="F55" s="26"/>
       <c r="G55" s="13"/>
-      <c r="H55" s="17"/>
+      <c r="H55" s="75"/>
       <c r="I55" s="13"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="17"/>
+      <c r="J55" s="75"/>
+      <c r="K55" s="13"/>
+      <c r="L55" s="75"/>
       <c r="M55" s="17"/>
       <c r="N55" s="19"/>
       <c r="O55" s="12"/>
@@ -5116,11 +5120,11 @@
       <c r="E56" s="25"/>
       <c r="F56" s="26"/>
       <c r="G56" s="13"/>
-      <c r="H56" s="17"/>
+      <c r="H56" s="75"/>
       <c r="I56" s="13"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="17"/>
+      <c r="J56" s="75"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="75"/>
       <c r="M56" s="17"/>
       <c r="N56" s="19"/>
       <c r="O56" s="12"/>
@@ -5141,44 +5145,44 @@
       <c r="J57" s="9"/>
     </row>
     <row r="58" spans="1:17">
-      <c r="B58" s="92" t="s">
+      <c r="B58" s="93" t="s">
         <v>103</v>
       </c>
-      <c r="C58" s="93"/>
-      <c r="D58" s="93"/>
-      <c r="E58" s="93"/>
-      <c r="F58" s="93"/>
-      <c r="G58" s="93"/>
-      <c r="H58" s="93"/>
-      <c r="I58" s="93"/>
-      <c r="J58" s="93"/>
-      <c r="K58" s="93"/>
-      <c r="L58" s="93"/>
-      <c r="M58" s="93"/>
-      <c r="N58" s="93"/>
-      <c r="O58" s="93"/>
-      <c r="P58" s="93"/>
-      <c r="Q58" s="93"/>
+      <c r="C58" s="94"/>
+      <c r="D58" s="94"/>
+      <c r="E58" s="94"/>
+      <c r="F58" s="94"/>
+      <c r="G58" s="94"/>
+      <c r="H58" s="94"/>
+      <c r="I58" s="94"/>
+      <c r="J58" s="94"/>
+      <c r="K58" s="94"/>
+      <c r="L58" s="94"/>
+      <c r="M58" s="94"/>
+      <c r="N58" s="94"/>
+      <c r="O58" s="94"/>
+      <c r="P58" s="94"/>
+      <c r="Q58" s="94"/>
     </row>
     <row r="59" spans="1:17">
-      <c r="B59" s="92" t="s">
+      <c r="B59" s="93" t="s">
         <v>104</v>
       </c>
-      <c r="C59" s="93"/>
-      <c r="D59" s="93"/>
-      <c r="E59" s="93"/>
-      <c r="F59" s="93"/>
-      <c r="G59" s="93"/>
-      <c r="H59" s="93"/>
-      <c r="I59" s="93"/>
-      <c r="J59" s="93"/>
-      <c r="K59" s="93"/>
-      <c r="L59" s="93"/>
-      <c r="M59" s="93"/>
-      <c r="N59" s="93"/>
-      <c r="O59" s="93"/>
-      <c r="P59" s="93"/>
-      <c r="Q59" s="93"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="94"/>
+      <c r="G59" s="94"/>
+      <c r="H59" s="94"/>
+      <c r="I59" s="94"/>
+      <c r="J59" s="94"/>
+      <c r="K59" s="94"/>
+      <c r="L59" s="94"/>
+      <c r="M59" s="94"/>
+      <c r="N59" s="94"/>
+      <c r="O59" s="94"/>
+      <c r="P59" s="94"/>
+      <c r="Q59" s="94"/>
     </row>
     <row r="62" spans="1:17">
       <c r="B62" s="1" t="s">
@@ -5291,10 +5295,10 @@
       <c r="L2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3" spans="1:16" s="16" customFormat="1">
       <c r="A3" s="2"/>
@@ -5315,42 +5319,42 @@
     </row>
     <row r="4" spans="1:16" s="16" customFormat="1" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="99"/>
-      <c r="C4" s="100" t="s">
+      <c r="B4" s="100"/>
+      <c r="C4" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="103" t="s">
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="104" t="s">
         <v>30</v>
       </c>
       <c r="P4" s="10"/>
     </row>
     <row r="5" spans="1:16" s="16" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="104" t="s">
+      <c r="B5" s="100"/>
+      <c r="C5" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="104" t="s">
+      <c r="D5" s="106"/>
+      <c r="E5" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="105"/>
-      <c r="G5" s="104" t="s">
+      <c r="F5" s="106"/>
+      <c r="G5" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="105"/>
-      <c r="I5" s="104" t="s">
+      <c r="H5" s="106"/>
+      <c r="I5" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="105"/>
-      <c r="K5" s="103"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="104"/>
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:16" s="16" customFormat="1" ht="16.149999999999999" customHeight="1">
@@ -5358,14 +5362,14 @@
       <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="106"/>
-      <c r="D6" s="107"/>
-      <c r="E6" s="106"/>
-      <c r="F6" s="107"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="109"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="110"/>
       <c r="K6" s="6"/>
       <c r="P6" s="10"/>
     </row>
@@ -5374,14 +5378,14 @@
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="106"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="108"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="109"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="110"/>
       <c r="K7" s="6"/>
       <c r="P7" s="10"/>
     </row>
@@ -5390,14 +5394,14 @@
       <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="107"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="108"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="108"/>
-      <c r="J8" s="109"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="107"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="110"/>
       <c r="K8" s="6"/>
       <c r="P8" s="10"/>
     </row>
@@ -5406,14 +5410,14 @@
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="106"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="109"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="109"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="110"/>
       <c r="K9" s="6"/>
       <c r="P9" s="10"/>
     </row>
@@ -5422,14 +5426,14 @@
       <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="108"/>
-      <c r="H10" s="109"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="109"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="110"/>
       <c r="K10" s="6"/>
       <c r="P10" s="10"/>
     </row>
@@ -5438,14 +5442,14 @@
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="106"/>
-      <c r="D11" s="107"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="108"/>
-      <c r="J11" s="109"/>
+      <c r="C11" s="107"/>
+      <c r="D11" s="108"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="110"/>
       <c r="K11" s="6"/>
       <c r="P11" s="10"/>
     </row>
@@ -5454,14 +5458,14 @@
       <c r="B12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="106"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="106"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="109"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="110"/>
       <c r="K12" s="6"/>
       <c r="L12" s="16"/>
       <c r="M12" s="16"/>
@@ -5474,14 +5478,14 @@
       <c r="B13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="106"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="108"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="108"/>
-      <c r="J13" s="109"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="108"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="108"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="110"/>
       <c r="K13" s="6"/>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
@@ -5494,14 +5498,14 @@
       <c r="B14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="106"/>
-      <c r="D14" s="107"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="107"/>
-      <c r="G14" s="108"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="108"/>
-      <c r="J14" s="109"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="110"/>
       <c r="K14" s="6"/>
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
@@ -5514,14 +5518,14 @@
       <c r="B15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="106"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="109"/>
+      <c r="C15" s="107"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="110"/>
       <c r="K15" s="6"/>
       <c r="L15" s="16"/>
       <c r="M15" s="16"/>
@@ -5689,69 +5693,69 @@
     </row>
     <row r="27" spans="1:16" s="3" customFormat="1" ht="16.149999999999999" customHeight="1">
       <c r="A27" s="2"/>
-      <c r="B27" s="110" t="s">
+      <c r="B27" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="110" t="s">
+      <c r="C27" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="D27" s="103" t="s">
+      <c r="D27" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="110" t="s">
+      <c r="E27" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="103" t="s">
+      <c r="F27" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="110" t="s">
+      <c r="G27" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="H27" s="103" t="s">
+      <c r="H27" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="110" t="s">
+      <c r="I27" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="J27" s="103" t="s">
+      <c r="J27" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="110" t="s">
+      <c r="K27" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="L27" s="103" t="s">
+      <c r="L27" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="M27" s="79" t="s">
+      <c r="M27" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="N27" s="103" t="s">
+      <c r="N27" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="O27" s="79" t="s">
+      <c r="O27" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="P27" s="103" t="s">
+      <c r="P27" s="104" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="3" customFormat="1" ht="17.25" customHeight="1">
       <c r="A28" s="2"/>
-      <c r="B28" s="111"/>
-      <c r="C28" s="111"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="103"/>
-      <c r="G28" s="111"/>
-      <c r="H28" s="103"/>
-      <c r="I28" s="111"/>
-      <c r="J28" s="103"/>
-      <c r="K28" s="111"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="80"/>
-      <c r="N28" s="103"/>
-      <c r="O28" s="80"/>
-      <c r="P28" s="103"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="112"/>
+      <c r="H28" s="104"/>
+      <c r="I28" s="112"/>
+      <c r="J28" s="104"/>
+      <c r="K28" s="112"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="104"/>
+      <c r="O28" s="82"/>
+      <c r="P28" s="104"/>
     </row>
     <row r="29" spans="1:16" s="3" customFormat="1">
       <c r="A29" s="2"/>
@@ -5886,32 +5890,32 @@
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="B37" s="110" t="s">
+      <c r="B37" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="110" t="s">
+      <c r="C37" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="D37" s="103" t="s">
+      <c r="D37" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="110" t="s">
+      <c r="F37" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="79" t="s">
+      <c r="G37" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="H37" s="103" t="s">
+      <c r="H37" s="104" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:16">
-      <c r="B38" s="111"/>
-      <c r="C38" s="111"/>
-      <c r="D38" s="103"/>
-      <c r="F38" s="111"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="103"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="104"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="104"/>
     </row>
     <row r="39" spans="1:16">
       <c r="B39" s="7" t="s">

</xml_diff>